<commit_message>
Documentatie sjabloom gemaakt & Vragenlijst
</commit_message>
<xml_diff>
--- a/go-nogo-formulier.xlsx
+++ b/go-nogo-formulier.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian\Documents\GitHub\Planning-PC4U-Website-MED1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeroen\Documents\GitHub\Planning-PC4U-Website-MED1\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="41">
   <si>
     <t>Week 1 : Oriëntatiefase</t>
   </si>
@@ -909,42 +909,42 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F157"/>
+  <dimension ref="A1:F140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="57.7109375" style="30" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" customWidth="1"/>
+    <col min="1" max="1" width="57.7265625" style="30" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="47.25" thickBot="1" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:6" ht="46.5" thickBot="1" x14ac:dyDescent="1.05">
       <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="39"/>
       <c r="C1" s="40"/>
     </row>
-    <row r="2" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" ht="29.25" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="43" t="s">
         <v>34</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
     </row>
-    <row r="3" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="43" t="s">
         <v>35</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
     </row>
-    <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>0</v>
       </c>
@@ -952,7 +952,7 @@
       <c r="C5" s="22"/>
       <c r="F5" s="1"/>
     </row>
-    <row r="6" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="14"/>
       <c r="B6" s="15" t="s">
         <v>1</v>
@@ -962,7 +962,7 @@
       </c>
       <c r="F6" s="1"/>
     </row>
-    <row r="7" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="14"/>
       <c r="B7" s="41" t="s">
         <v>3</v>
@@ -972,7 +972,7 @@
       </c>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="14"/>
       <c r="B8" s="16" t="s">
         <v>4</v>
@@ -982,7 +982,7 @@
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="14"/>
       <c r="B9" s="18" t="s">
         <v>6</v>
@@ -991,21 +991,21 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
         <v>40</v>
       </c>
       <c r="B10" s="24"/>
       <c r="C10" s="25"/>
     </row>
-    <row r="11" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="32" t="s">
         <v>37</v>
       </c>
       <c r="B11" s="26"/>
       <c r="C11" s="27"/>
     </row>
-    <row r="12" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="32" t="s">
         <v>39</v>
       </c>
@@ -1013,60 +1013,60 @@
       <c r="C12" s="27"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="32" t="s">
         <v>36</v>
       </c>
       <c r="B13" s="26"/>
       <c r="C13" s="27"/>
     </row>
-    <row r="14" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="33" t="s">
         <v>38</v>
       </c>
       <c r="B14" s="28"/>
       <c r="C14" s="29"/>
     </row>
-    <row r="15" spans="1:6" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="10"/>
       <c r="C16" s="11"/>
     </row>
-    <row r="17" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="34"/>
       <c r="B17" s="6"/>
       <c r="C17" s="4"/>
     </row>
-    <row r="18" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6"/>
       <c r="C18" s="4"/>
     </row>
-    <row r="19" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="5"/>
       <c r="C19" s="12"/>
     </row>
-    <row r="20" spans="1:3" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="35"/>
       <c r="B20" s="20"/>
       <c r="C20" s="20"/>
     </row>
-    <row r="21" spans="1:3" ht="24.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="35"/>
       <c r="B21" s="20"/>
       <c r="C21" s="20"/>
     </row>
-    <row r="22" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="21"/>
       <c r="C22" s="22"/>
     </row>
-    <row r="23" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="9"/>
       <c r="B23" s="2" t="s">
         <v>1</v>
@@ -1075,7 +1075,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="14"/>
       <c r="B24" s="41" t="s">
         <v>3</v>
@@ -1084,7 +1084,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="14"/>
       <c r="B25" s="16" t="s">
         <v>4</v>
@@ -1093,7 +1093,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="14"/>
       <c r="B26" s="18" t="s">
         <v>6</v>
@@ -1102,77 +1102,77 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B27" s="24"/>
       <c r="C27" s="25"/>
     </row>
-    <row r="28" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="32" t="s">
         <v>10</v>
       </c>
       <c r="B28" s="26"/>
       <c r="C28" s="27"/>
     </row>
-    <row r="29" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B29" s="26"/>
       <c r="C29" s="27"/>
     </row>
-    <row r="30" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="32"/>
       <c r="B30" s="26"/>
       <c r="C30" s="27"/>
     </row>
-    <row r="31" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="33"/>
       <c r="B31" s="28"/>
       <c r="C31" s="29"/>
     </row>
-    <row r="32" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="10"/>
       <c r="C33" s="11"/>
     </row>
-    <row r="34" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="34"/>
       <c r="B34" s="6"/>
       <c r="C34" s="4"/>
     </row>
-    <row r="35" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="6"/>
       <c r="C35" s="4"/>
     </row>
-    <row r="36" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B36" s="5"/>
       <c r="C36" s="12"/>
     </row>
-    <row r="37" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="35"/>
       <c r="B37" s="20"/>
       <c r="C37" s="20"/>
     </row>
-    <row r="38" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="35"/>
       <c r="B38" s="20"/>
       <c r="C38" s="20"/>
     </row>
-    <row r="39" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B39" s="21"/>
       <c r="C39" s="22"/>
     </row>
-    <row r="40" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="9"/>
       <c r="B40" s="2" t="s">
         <v>1</v>
@@ -1181,7 +1181,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="14"/>
       <c r="B41" s="41" t="s">
         <v>3</v>
@@ -1190,7 +1190,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="14"/>
       <c r="B42" s="16" t="s">
         <v>4</v>
@@ -1199,7 +1199,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="14"/>
       <c r="B43" s="18" t="s">
         <v>6</v>
@@ -1208,81 +1208,81 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="31" t="s">
         <v>13</v>
       </c>
       <c r="B44" s="24"/>
       <c r="C44" s="25"/>
     </row>
-    <row r="45" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="36" t="s">
         <v>14</v>
       </c>
       <c r="B45" s="26"/>
       <c r="C45" s="27"/>
     </row>
-    <row r="46" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="37" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="26"/>
       <c r="C46" s="27"/>
     </row>
-    <row r="47" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B47" s="26"/>
       <c r="C47" s="27"/>
     </row>
-    <row r="48" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B48" s="28"/>
       <c r="C48" s="29"/>
     </row>
-    <row r="49" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B49" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B50" s="10"/>
       <c r="C50" s="11"/>
     </row>
-    <row r="51" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="34"/>
       <c r="B51" s="6"/>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B52" s="6"/>
       <c r="C52" s="4"/>
     </row>
-    <row r="53" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B53" s="5"/>
       <c r="C53" s="12"/>
     </row>
-    <row r="54" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="35"/>
       <c r="B54" s="20"/>
       <c r="C54" s="20"/>
     </row>
-    <row r="55" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="35"/>
       <c r="B55" s="20"/>
       <c r="C55" s="20"/>
     </row>
-    <row r="56" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>17</v>
       </c>
       <c r="B56" s="21"/>
       <c r="C56" s="22"/>
     </row>
-    <row r="57" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B57" s="2" t="s">
         <v>1</v>
       </c>
@@ -1290,7 +1290,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="14"/>
       <c r="B58" s="41" t="s">
         <v>3</v>
@@ -1299,7 +1299,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="14"/>
       <c r="B59" s="16" t="s">
         <v>4</v>
@@ -1308,7 +1308,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="14"/>
       <c r="B60" s="18" t="s">
         <v>6</v>
@@ -1317,79 +1317,82 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="31" t="s">
         <v>18</v>
       </c>
       <c r="B61" s="24"/>
       <c r="C61" s="25"/>
     </row>
-    <row r="62" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="36" t="s">
         <v>19</v>
       </c>
       <c r="B62" s="26"/>
       <c r="C62" s="27"/>
     </row>
-    <row r="63" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="37"/>
       <c r="B63" s="26"/>
       <c r="C63" s="27"/>
     </row>
-    <row r="64" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B64" s="26"/>
       <c r="C64" s="27"/>
     </row>
-    <row r="65" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B65" s="28"/>
       <c r="C65" s="29"/>
     </row>
-    <row r="66" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B66" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B67" s="10"/>
       <c r="C67" s="11"/>
     </row>
-    <row r="68" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="34"/>
       <c r="B68" s="6"/>
       <c r="C68" s="4"/>
     </row>
-    <row r="69" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B69" s="6"/>
       <c r="C69" s="4"/>
     </row>
-    <row r="70" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B70" s="5"/>
       <c r="C70" s="12"/>
     </row>
-    <row r="71" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="35"/>
       <c r="B71" s="20"/>
       <c r="C71" s="20"/>
     </row>
-    <row r="72" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="35"/>
       <c r="B72" s="20"/>
       <c r="C72" s="20"/>
     </row>
-    <row r="73" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="7" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B73" s="21"/>
       <c r="C73" s="22"/>
     </row>
-    <row r="74" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A74" s="34" t="s">
+        <v>24</v>
+      </c>
       <c r="B74" s="2" t="s">
         <v>1</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="14"/>
       <c r="B75" s="41" t="s">
         <v>3</v>
@@ -1406,7 +1409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="14"/>
       <c r="B76" s="16" t="s">
         <v>4</v>
@@ -1415,7 +1418,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="14"/>
       <c r="B77" s="18" t="s">
         <v>6</v>
@@ -1424,82 +1427,82 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="31" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B78" s="24"/>
       <c r="C78" s="25"/>
     </row>
-    <row r="79" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="36" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B79" s="26"/>
       <c r="C79" s="27"/>
     </row>
-    <row r="80" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="37"/>
+    <row r="80" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="37" t="s">
+        <v>23</v>
+      </c>
       <c r="B80" s="26"/>
       <c r="C80" s="27"/>
     </row>
-    <row r="81" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B81" s="26"/>
       <c r="C81" s="27"/>
     </row>
-    <row r="82" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A82" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B82" s="28"/>
       <c r="C82" s="29"/>
     </row>
-    <row r="83" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B83" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B84" s="10"/>
       <c r="C84" s="11"/>
     </row>
-    <row r="85" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="34"/>
       <c r="B85" s="6"/>
       <c r="C85" s="4"/>
     </row>
-    <row r="86" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B86" s="6"/>
       <c r="C86" s="4"/>
     </row>
-    <row r="87" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B87" s="5"/>
       <c r="C87" s="12"/>
     </row>
-    <row r="88" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="35"/>
       <c r="B88" s="20"/>
       <c r="C88" s="20"/>
     </row>
-    <row r="89" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A89" s="35"/>
       <c r="B89" s="20"/>
       <c r="C89" s="20"/>
     </row>
-    <row r="90" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="7" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="B90" s="21"/>
       <c r="C90" s="22"/>
     </row>
-    <row r="91" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="34" t="s">
-        <v>24</v>
-      </c>
+    <row r="91" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="34"/>
       <c r="B91" s="2" t="s">
         <v>1</v>
       </c>
@@ -1507,7 +1510,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="92" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="14"/>
       <c r="B92" s="41" t="s">
         <v>3</v>
@@ -1516,7 +1519,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="93" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="14"/>
       <c r="B93" s="16" t="s">
         <v>4</v>
@@ -1525,7 +1528,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="94" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="14"/>
       <c r="B94" s="18" t="s">
         <v>6</v>
@@ -1534,81 +1537,79 @@
         <v>6</v>
       </c>
     </row>
-    <row r="95" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="31" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="B95" s="24"/>
       <c r="C95" s="25"/>
     </row>
-    <row r="96" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="36" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B96" s="26"/>
       <c r="C96" s="27"/>
     </row>
-    <row r="97" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A97" s="37" t="s">
-        <v>23</v>
-      </c>
+    <row r="97" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A97" s="37"/>
       <c r="B97" s="26"/>
       <c r="C97" s="27"/>
     </row>
-    <row r="98" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="32" t="s">
         <v>11</v>
       </c>
       <c r="B98" s="26"/>
       <c r="C98" s="27"/>
     </row>
-    <row r="99" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="33" t="s">
         <v>15</v>
       </c>
       <c r="B99" s="28"/>
       <c r="C99" s="29"/>
     </row>
-    <row r="100" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B100" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="101" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B101" s="10"/>
       <c r="C101" s="11"/>
     </row>
-    <row r="102" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A102" s="34"/>
       <c r="B102" s="6"/>
       <c r="C102" s="4"/>
     </row>
-    <row r="103" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B103" s="6"/>
       <c r="C103" s="4"/>
     </row>
-    <row r="104" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B104" s="5"/>
       <c r="C104" s="12"/>
     </row>
-    <row r="105" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A105" s="35"/>
       <c r="B105" s="20"/>
       <c r="C105" s="20"/>
     </row>
-    <row r="106" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A106" s="35"/>
       <c r="B106" s="20"/>
       <c r="C106" s="20"/>
     </row>
-    <row r="107" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A107" s="7" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B107" s="21"/>
       <c r="C107" s="22"/>
     </row>
-    <row r="108" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A108" s="34"/>
       <c r="B108" s="2" t="s">
         <v>1</v>
@@ -1617,7 +1618,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A109" s="14"/>
       <c r="B109" s="41" t="s">
         <v>3</v>
@@ -1626,7 +1627,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A110" s="14"/>
       <c r="B110" s="16" t="s">
         <v>4</v>
@@ -1635,7 +1636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A111" s="14"/>
       <c r="B111" s="18" t="s">
         <v>6</v>
@@ -1644,282 +1645,174 @@
         <v>6</v>
       </c>
     </row>
-    <row r="112" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A112" s="31" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B112" s="24"/>
       <c r="C112" s="25"/>
     </row>
-    <row r="113" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A113" s="36" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B113" s="26"/>
       <c r="C113" s="27"/>
     </row>
-    <row r="114" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A114" s="37"/>
+    <row r="114" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A114" s="36" t="s">
+        <v>32</v>
+      </c>
       <c r="B114" s="26"/>
       <c r="C114" s="27"/>
     </row>
-    <row r="115" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A115" s="32" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="B115" s="26"/>
       <c r="C115" s="27"/>
     </row>
-    <row r="116" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A116" s="33" t="s">
+    <row r="116" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A116" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="B116" s="26"/>
+      <c r="C116" s="27"/>
+    </row>
+    <row r="117" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="B116" s="28"/>
-      <c r="C116" s="29"/>
-    </row>
-    <row r="117" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B117" s="1" t="s">
+      <c r="B117" s="28"/>
+      <c r="C117" s="29"/>
+    </row>
+    <row r="118" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B118" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B118" s="10"/>
-      <c r="C118" s="11"/>
-    </row>
-    <row r="119" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="34"/>
-      <c r="B119" s="6"/>
-      <c r="C119" s="4"/>
-    </row>
-    <row r="120" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B119" s="10"/>
+      <c r="C119" s="11"/>
+    </row>
+    <row r="120" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A120" s="34"/>
       <c r="B120" s="6"/>
       <c r="C120" s="4"/>
     </row>
-    <row r="121" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B121" s="5"/>
-      <c r="C121" s="12"/>
-    </row>
-    <row r="122" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A122" s="35"/>
-      <c r="B122" s="20"/>
-      <c r="C122" s="20"/>
-    </row>
-    <row r="123" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B121" s="6"/>
+      <c r="C121" s="4"/>
+    </row>
+    <row r="122" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B122" s="5"/>
+      <c r="C122" s="12"/>
+    </row>
+    <row r="123" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A123" s="35"/>
       <c r="B123" s="20"/>
       <c r="C123" s="20"/>
     </row>
-    <row r="124" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A124" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="B124" s="21"/>
-      <c r="C124" s="22"/>
-    </row>
-    <row r="125" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="34"/>
-      <c r="B125" s="2" t="s">
+    <row r="124" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A124" s="35"/>
+      <c r="B124" s="20"/>
+      <c r="C124" s="20"/>
+    </row>
+    <row r="125" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A125" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B125" s="21"/>
+      <c r="C125" s="22"/>
+    </row>
+    <row r="126" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A126" s="34"/>
+      <c r="B126" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C125" s="3" t="s">
+      <c r="C126" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="126" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A126" s="14"/>
-      <c r="B126" s="41" t="s">
+    <row r="127" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A127" s="14"/>
+      <c r="B127" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="C126" s="42" t="s">
+      <c r="C127" s="42" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A127" s="14"/>
-      <c r="B127" s="16" t="s">
+    <row r="128" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A128" s="14"/>
+      <c r="B128" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C127" s="17" t="s">
+      <c r="C128" s="17" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A128" s="14"/>
-      <c r="B128" s="18" t="s">
+    <row r="129" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A129" s="14"/>
+      <c r="B129" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="C128" s="19" t="s">
+      <c r="C129" s="19" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A129" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B129" s="24"/>
-      <c r="C129" s="25"/>
-    </row>
-    <row r="130" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A130" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="B130" s="26"/>
-      <c r="C130" s="27"/>
-    </row>
-    <row r="131" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A131" s="36" t="s">
-        <v>32</v>
-      </c>
+    <row r="130" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="31"/>
+      <c r="B130" s="24"/>
+      <c r="C130" s="25"/>
+    </row>
+    <row r="131" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A131" s="36"/>
       <c r="B131" s="26"/>
       <c r="C131" s="27"/>
     </row>
-    <row r="132" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A132" s="32" t="s">
-        <v>31</v>
-      </c>
+    <row r="132" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A132" s="36"/>
       <c r="B132" s="26"/>
       <c r="C132" s="27"/>
     </row>
-    <row r="133" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="32" t="s">
-        <v>11</v>
-      </c>
+    <row r="133" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A133" s="32"/>
       <c r="B133" s="26"/>
       <c r="C133" s="27"/>
     </row>
-    <row r="134" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A134" s="33" t="s">
-        <v>15</v>
-      </c>
-      <c r="B134" s="28"/>
-      <c r="C134" s="29"/>
-    </row>
-    <row r="135" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B135" s="1" t="s">
+    <row r="134" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A134" s="32"/>
+      <c r="B134" s="26"/>
+      <c r="C134" s="27"/>
+    </row>
+    <row r="135" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A135" s="33"/>
+      <c r="B135" s="28"/>
+      <c r="C135" s="29"/>
+    </row>
+    <row r="136" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B136" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B136" s="10"/>
-      <c r="C136" s="11"/>
-    </row>
-    <row r="137" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A137" s="34"/>
-      <c r="B137" s="6"/>
-      <c r="C137" s="4"/>
-    </row>
-    <row r="138" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B137" s="10"/>
+      <c r="C137" s="11"/>
+    </row>
+    <row r="138" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="34"/>
       <c r="B138" s="6"/>
       <c r="C138" s="4"/>
     </row>
-    <row r="139" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B139" s="5"/>
-      <c r="C139" s="12"/>
-    </row>
-    <row r="140" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A140" s="35"/>
-      <c r="B140" s="20"/>
-      <c r="C140" s="20"/>
-    </row>
-    <row r="141" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="35"/>
-      <c r="B141" s="20"/>
-      <c r="C141" s="20"/>
-    </row>
-    <row r="142" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A142" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B142" s="21"/>
-      <c r="C142" s="22"/>
-    </row>
-    <row r="143" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="34"/>
-      <c r="B143" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C143" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="144" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="14"/>
-      <c r="B144" s="41" t="s">
-        <v>3</v>
-      </c>
-      <c r="C144" s="42" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="14"/>
-      <c r="B145" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C145" s="17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="14"/>
-      <c r="B146" s="18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C146" s="19" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="147" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A147" s="31"/>
-      <c r="B147" s="24"/>
-      <c r="C147" s="25"/>
-    </row>
-    <row r="148" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A148" s="36"/>
-      <c r="B148" s="26"/>
-      <c r="C148" s="27"/>
-    </row>
-    <row r="149" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="36"/>
-      <c r="B149" s="26"/>
-      <c r="C149" s="27"/>
-    </row>
-    <row r="150" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A150" s="32"/>
-      <c r="B150" s="26"/>
-      <c r="C150" s="27"/>
-    </row>
-    <row r="151" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A151" s="32"/>
-      <c r="B151" s="26"/>
-      <c r="C151" s="27"/>
-    </row>
-    <row r="152" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="33"/>
-      <c r="B152" s="28"/>
-      <c r="C152" s="29"/>
-    </row>
-    <row r="153" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B153" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B154" s="10"/>
-      <c r="C154" s="11"/>
-    </row>
-    <row r="155" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A155" s="34"/>
-      <c r="B155" s="6"/>
-      <c r="C155" s="4"/>
-    </row>
-    <row r="156" spans="1:3" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B156" s="6"/>
-      <c r="C156" s="4"/>
-    </row>
-    <row r="157" spans="1:3" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B157" s="5"/>
-      <c r="C157" s="12"/>
+    <row r="139" spans="1:3" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B139" s="6"/>
+      <c r="C139" s="4"/>
+    </row>
+    <row r="140" spans="1:3" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B140" s="5"/>
+      <c r="C140" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1928,6 +1821,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101007BEF67E862DF8142A1371705B0F69A4C" ma:contentTypeVersion="0" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="649c850f7c3b7898c616adec0832281d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b118b0825d757084c8d1e1ffd33f200c">
     <xsd:element name="properties">
@@ -1976,12 +1875,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1992,6 +1885,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F2FB8B0-C61D-4AED-9816-2F0F1A6E555A}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C4ABFC39-04E8-48CD-9F55-12A5635B9619}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2006,20 +1913,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F2FB8B0-C61D-4AED-9816-2F0F1A6E555A}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2373A8D6-0915-48B0-9DFB-3BBCFE9FF3C6}">
   <ds:schemaRefs>

</xml_diff>